<commit_message>
Update Experimentation Results_4 UCAV,6 Targets(3AA,1APC,2Tanks).xlsx
</commit_message>
<xml_diff>
--- a/data/Experimentation Results_4 UCAV,6 Targets(3AA,1APC,2Tanks).xlsx
+++ b/data/Experimentation Results_4 UCAV,6 Targets(3AA,1APC,2Tanks).xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21425"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84FEC93F-633B-49FB-AE14-BC8184D80A18}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F11429E4-76BC-45E8-94DA-71FB72963628}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="6165" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="6165" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Experiments" sheetId="1" r:id="rId1"/>
@@ -528,68 +528,68 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -873,8 +873,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N92"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E53" workbookViewId="0">
-      <selection activeCell="L48" sqref="L48:L71"/>
+    <sheetView topLeftCell="E19" workbookViewId="0">
+      <selection activeCell="K9" sqref="K9:K38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -895,109 +895,109 @@
     <col min="14" max="14" width="16.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="46" customFormat="1" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="46" t="s">
+    <row r="1" spans="1:14" s="65" customFormat="1" ht="21" x14ac:dyDescent="0.35">
+      <c r="A1" s="65" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="47" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="47" t="s">
+    <row r="2" spans="1:14" s="66" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="66" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:14" s="48" customFormat="1" ht="19.5" x14ac:dyDescent="0.3">
-      <c r="A4" s="48" t="s">
+    <row r="4" spans="1:14" s="59" customFormat="1" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="A4" s="59" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
-      <c r="B5" s="49" t="s">
+      <c r="B5" s="60" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="50"/>
-      <c r="D5" s="50"/>
-      <c r="E5" s="50"/>
-      <c r="F5" s="50"/>
-      <c r="H5" s="51" t="s">
-        <v>1</v>
-      </c>
-      <c r="I5" s="51"/>
-      <c r="J5" s="51"/>
-      <c r="K5" s="51"/>
-      <c r="L5" s="51"/>
+      <c r="C5" s="61"/>
+      <c r="D5" s="61"/>
+      <c r="E5" s="61"/>
+      <c r="F5" s="61"/>
+      <c r="H5" s="62" t="s">
+        <v>1</v>
+      </c>
+      <c r="I5" s="62"/>
+      <c r="J5" s="62"/>
+      <c r="K5" s="62"/>
+      <c r="L5" s="62"/>
       <c r="M5" s="2"/>
     </row>
     <row r="6" spans="1:14" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="52" t="s">
-        <v>2</v>
-      </c>
-      <c r="B6" s="55" t="s">
-        <v>3</v>
-      </c>
-      <c r="C6" s="55" t="s">
+      <c r="A6" s="63" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" s="58" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="58" t="s">
         <v>26</v>
       </c>
-      <c r="D6" s="55" t="s">
-        <v>4</v>
-      </c>
-      <c r="E6" s="55" t="s">
-        <v>5</v>
-      </c>
-      <c r="F6" s="58" t="s">
-        <v>6</v>
-      </c>
-      <c r="H6" s="61" t="s">
+      <c r="D6" s="58" t="s">
+        <v>4</v>
+      </c>
+      <c r="E6" s="58" t="s">
+        <v>5</v>
+      </c>
+      <c r="F6" s="49" t="s">
+        <v>6</v>
+      </c>
+      <c r="H6" s="52" t="s">
         <v>7</v>
       </c>
-      <c r="I6" s="64" t="s">
+      <c r="I6" s="55" t="s">
         <v>27</v>
       </c>
-      <c r="J6" s="64" t="s">
+      <c r="J6" s="55" t="s">
         <v>19</v>
       </c>
-      <c r="K6" s="64" t="s">
+      <c r="K6" s="55" t="s">
         <v>14</v>
       </c>
-      <c r="L6" s="55" t="s">
+      <c r="L6" s="58" t="s">
         <v>21</v>
       </c>
-      <c r="M6" s="56" t="s">
+      <c r="M6" s="46" t="s">
         <v>20</v>
       </c>
-      <c r="N6" s="58" t="s">
+      <c r="N6" s="49" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="53"/>
-      <c r="B7" s="56"/>
-      <c r="C7" s="56"/>
-      <c r="D7" s="56"/>
-      <c r="E7" s="53"/>
-      <c r="F7" s="59"/>
-      <c r="H7" s="62"/>
-      <c r="I7" s="65"/>
-      <c r="J7" s="65"/>
-      <c r="K7" s="65"/>
-      <c r="L7" s="53"/>
-      <c r="M7" s="53"/>
-      <c r="N7" s="59"/>
+      <c r="A7" s="47"/>
+      <c r="B7" s="46"/>
+      <c r="C7" s="46"/>
+      <c r="D7" s="46"/>
+      <c r="E7" s="47"/>
+      <c r="F7" s="50"/>
+      <c r="H7" s="53"/>
+      <c r="I7" s="56"/>
+      <c r="J7" s="56"/>
+      <c r="K7" s="56"/>
+      <c r="L7" s="47"/>
+      <c r="M7" s="47"/>
+      <c r="N7" s="50"/>
     </row>
     <row r="8" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="54"/>
-      <c r="B8" s="57"/>
-      <c r="C8" s="57"/>
-      <c r="D8" s="57"/>
-      <c r="E8" s="54"/>
-      <c r="F8" s="60"/>
-      <c r="H8" s="63"/>
-      <c r="I8" s="66"/>
-      <c r="J8" s="66"/>
-      <c r="K8" s="66"/>
-      <c r="L8" s="54"/>
-      <c r="M8" s="54"/>
-      <c r="N8" s="60"/>
+      <c r="A8" s="48"/>
+      <c r="B8" s="64"/>
+      <c r="C8" s="64"/>
+      <c r="D8" s="64"/>
+      <c r="E8" s="48"/>
+      <c r="F8" s="51"/>
+      <c r="H8" s="54"/>
+      <c r="I8" s="57"/>
+      <c r="J8" s="57"/>
+      <c r="K8" s="57"/>
+      <c r="L8" s="48"/>
+      <c r="M8" s="48"/>
+      <c r="N8" s="51"/>
     </row>
     <row r="9" spans="1:14" s="37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="9">
@@ -2279,99 +2279,99 @@
       <c r="J41" s="8"/>
       <c r="K41" s="8"/>
     </row>
-    <row r="42" spans="1:14" s="48" customFormat="1" ht="19.5" x14ac:dyDescent="0.3">
-      <c r="A42" s="48" t="s">
+    <row r="42" spans="1:14" s="59" customFormat="1" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="A42" s="59" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="43" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="1"/>
-      <c r="B43" s="49" t="s">
+      <c r="B43" s="60" t="s">
         <v>0</v>
       </c>
-      <c r="C43" s="50"/>
-      <c r="D43" s="50"/>
-      <c r="E43" s="50"/>
-      <c r="F43" s="50"/>
-      <c r="H43" s="51" t="s">
-        <v>1</v>
-      </c>
-      <c r="I43" s="51"/>
-      <c r="J43" s="51"/>
-      <c r="K43" s="51"/>
-      <c r="L43" s="51"/>
+      <c r="C43" s="61"/>
+      <c r="D43" s="61"/>
+      <c r="E43" s="61"/>
+      <c r="F43" s="61"/>
+      <c r="H43" s="62" t="s">
+        <v>1</v>
+      </c>
+      <c r="I43" s="62"/>
+      <c r="J43" s="62"/>
+      <c r="K43" s="62"/>
+      <c r="L43" s="62"/>
       <c r="M43" s="2"/>
     </row>
     <row r="44" spans="1:14" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="52" t="s">
-        <v>2</v>
-      </c>
-      <c r="B44" s="55" t="s">
-        <v>3</v>
-      </c>
-      <c r="C44" s="55" t="s">
+      <c r="A44" s="63" t="s">
+        <v>2</v>
+      </c>
+      <c r="B44" s="58" t="s">
+        <v>3</v>
+      </c>
+      <c r="C44" s="58" t="s">
         <v>26</v>
       </c>
-      <c r="D44" s="55" t="s">
-        <v>4</v>
-      </c>
-      <c r="E44" s="55" t="s">
-        <v>5</v>
-      </c>
-      <c r="F44" s="58" t="s">
-        <v>6</v>
-      </c>
-      <c r="H44" s="61" t="s">
+      <c r="D44" s="58" t="s">
+        <v>4</v>
+      </c>
+      <c r="E44" s="58" t="s">
+        <v>5</v>
+      </c>
+      <c r="F44" s="49" t="s">
+        <v>6</v>
+      </c>
+      <c r="H44" s="52" t="s">
         <v>7</v>
       </c>
-      <c r="I44" s="64" t="s">
+      <c r="I44" s="55" t="s">
         <v>27</v>
       </c>
-      <c r="J44" s="64" t="s">
+      <c r="J44" s="55" t="s">
         <v>19</v>
       </c>
-      <c r="K44" s="64" t="s">
+      <c r="K44" s="55" t="s">
         <v>14</v>
       </c>
-      <c r="L44" s="55" t="s">
+      <c r="L44" s="58" t="s">
         <v>21</v>
       </c>
-      <c r="M44" s="56" t="s">
+      <c r="M44" s="46" t="s">
         <v>20</v>
       </c>
-      <c r="N44" s="58" t="s">
+      <c r="N44" s="49" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="45" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="53"/>
-      <c r="B45" s="56"/>
-      <c r="C45" s="56"/>
-      <c r="D45" s="56"/>
-      <c r="E45" s="53"/>
-      <c r="F45" s="59"/>
-      <c r="H45" s="62"/>
-      <c r="I45" s="65"/>
-      <c r="J45" s="65"/>
-      <c r="K45" s="65"/>
-      <c r="L45" s="53"/>
-      <c r="M45" s="53"/>
-      <c r="N45" s="59"/>
+      <c r="A45" s="47"/>
+      <c r="B45" s="46"/>
+      <c r="C45" s="46"/>
+      <c r="D45" s="46"/>
+      <c r="E45" s="47"/>
+      <c r="F45" s="50"/>
+      <c r="H45" s="53"/>
+      <c r="I45" s="56"/>
+      <c r="J45" s="56"/>
+      <c r="K45" s="56"/>
+      <c r="L45" s="47"/>
+      <c r="M45" s="47"/>
+      <c r="N45" s="50"/>
     </row>
     <row r="46" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="54"/>
-      <c r="B46" s="57"/>
-      <c r="C46" s="57"/>
-      <c r="D46" s="57"/>
-      <c r="E46" s="54"/>
-      <c r="F46" s="60"/>
-      <c r="H46" s="63"/>
-      <c r="I46" s="66"/>
-      <c r="J46" s="66"/>
-      <c r="K46" s="66"/>
-      <c r="L46" s="54"/>
-      <c r="M46" s="54"/>
-      <c r="N46" s="60"/>
+      <c r="A46" s="48"/>
+      <c r="B46" s="64"/>
+      <c r="C46" s="64"/>
+      <c r="D46" s="64"/>
+      <c r="E46" s="48"/>
+      <c r="F46" s="51"/>
+      <c r="H46" s="54"/>
+      <c r="I46" s="57"/>
+      <c r="J46" s="57"/>
+      <c r="K46" s="57"/>
+      <c r="L46" s="48"/>
+      <c r="M46" s="48"/>
+      <c r="N46" s="51"/>
     </row>
     <row r="47" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="9">
@@ -3733,14 +3733,16 @@
     </row>
   </sheetData>
   <mergeCells count="34">
-    <mergeCell ref="M44:M46"/>
-    <mergeCell ref="N44:N46"/>
-    <mergeCell ref="F44:F46"/>
-    <mergeCell ref="H44:H46"/>
-    <mergeCell ref="I44:I46"/>
-    <mergeCell ref="J44:J46"/>
-    <mergeCell ref="K44:K46"/>
-    <mergeCell ref="L44:L46"/>
+    <mergeCell ref="A1:XFD1"/>
+    <mergeCell ref="A2:XFD2"/>
+    <mergeCell ref="A4:XFD4"/>
+    <mergeCell ref="B5:F5"/>
+    <mergeCell ref="H5:L5"/>
+    <mergeCell ref="A44:A46"/>
+    <mergeCell ref="B44:B46"/>
+    <mergeCell ref="C44:C46"/>
+    <mergeCell ref="D44:D46"/>
+    <mergeCell ref="E44:E46"/>
     <mergeCell ref="M6:M8"/>
     <mergeCell ref="N6:N8"/>
     <mergeCell ref="A42:XFD42"/>
@@ -3757,16 +3759,14 @@
     <mergeCell ref="C6:C8"/>
     <mergeCell ref="D6:D8"/>
     <mergeCell ref="E6:E8"/>
-    <mergeCell ref="A44:A46"/>
-    <mergeCell ref="B44:B46"/>
-    <mergeCell ref="C44:C46"/>
-    <mergeCell ref="D44:D46"/>
-    <mergeCell ref="E44:E46"/>
-    <mergeCell ref="A1:XFD1"/>
-    <mergeCell ref="A2:XFD2"/>
-    <mergeCell ref="A4:XFD4"/>
-    <mergeCell ref="B5:F5"/>
-    <mergeCell ref="H5:L5"/>
+    <mergeCell ref="M44:M46"/>
+    <mergeCell ref="N44:N46"/>
+    <mergeCell ref="F44:F46"/>
+    <mergeCell ref="H44:H46"/>
+    <mergeCell ref="I44:I46"/>
+    <mergeCell ref="J44:J46"/>
+    <mergeCell ref="K44:K46"/>
+    <mergeCell ref="L44:L46"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3777,8 +3777,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA9998C4-CC4C-4D96-A9F6-38D1D124CD8B}">
   <dimension ref="A1:L32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E33" sqref="E33"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3846,7 +3846,7 @@
         <v>266</v>
       </c>
       <c r="G2" s="8">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="H2" s="8">
         <v>10</v>
@@ -3884,7 +3884,7 @@
         <v>247</v>
       </c>
       <c r="G3" s="8">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="H3" s="8">
         <v>4</v>
@@ -3922,7 +3922,7 @@
         <v>1010</v>
       </c>
       <c r="G4" s="8">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="H4" s="8">
         <v>11</v>
@@ -3960,7 +3960,7 @@
         <v>330</v>
       </c>
       <c r="G5" s="8">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="H5" s="8">
         <v>6</v>
@@ -3998,7 +3998,7 @@
         <v>420</v>
       </c>
       <c r="G6" s="8">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="H6" s="8">
         <v>3</v>
@@ -4036,7 +4036,7 @@
         <v>460</v>
       </c>
       <c r="G7" s="8">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="H7" s="8">
         <v>6</v>
@@ -4074,7 +4074,7 @@
         <v>541</v>
       </c>
       <c r="G8" s="8">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H8" s="8">
         <v>12</v>
@@ -4112,7 +4112,7 @@
         <v>470</v>
       </c>
       <c r="G9" s="8">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="H9" s="8">
         <v>9</v>
@@ -4150,7 +4150,7 @@
         <v>455</v>
       </c>
       <c r="G10" s="8">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="H10" s="8">
         <v>4</v>
@@ -4188,7 +4188,7 @@
         <v>442</v>
       </c>
       <c r="G11" s="8">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H11" s="8">
         <v>7</v>
@@ -4226,7 +4226,7 @@
         <v>434</v>
       </c>
       <c r="G12" s="8">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="H12" s="8">
         <v>6</v>
@@ -4264,7 +4264,7 @@
         <v>414</v>
       </c>
       <c r="G13" s="8">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="H13" s="8">
         <v>12</v>
@@ -4302,7 +4302,7 @@
         <v>653</v>
       </c>
       <c r="G14" s="13">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="H14" s="13">
         <v>12</v>
@@ -4340,7 +4340,7 @@
         <v>259</v>
       </c>
       <c r="G15" s="8">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="H15" s="8">
         <v>3</v>
@@ -4378,7 +4378,7 @@
         <v>345</v>
       </c>
       <c r="G16" s="8">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="H16" s="8">
         <v>4</v>
@@ -4416,7 +4416,7 @@
         <v>243</v>
       </c>
       <c r="G17" s="8">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="H17" s="8">
         <v>3</v>
@@ -4454,7 +4454,7 @@
         <v>347</v>
       </c>
       <c r="G18" s="8">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="H18" s="8">
         <v>5</v>
@@ -4492,7 +4492,7 @@
         <v>535</v>
       </c>
       <c r="G19" s="8">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H19" s="8">
         <v>7</v>
@@ -4530,7 +4530,7 @@
         <v>641</v>
       </c>
       <c r="G20" s="8">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="H20" s="8">
         <v>5</v>
@@ -4568,7 +4568,7 @@
         <v>202</v>
       </c>
       <c r="G21" s="8">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="H21" s="8">
         <v>2</v>
@@ -4606,7 +4606,7 @@
         <v>547</v>
       </c>
       <c r="G22" s="8">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="H22" s="8">
         <v>4</v>
@@ -4644,7 +4644,7 @@
         <v>436</v>
       </c>
       <c r="G23" s="8">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="H23" s="8">
         <v>8</v>
@@ -4682,7 +4682,7 @@
         <v>388</v>
       </c>
       <c r="G24" s="8">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="H24" s="8">
         <v>9</v>
@@ -4720,7 +4720,7 @@
         <v>337</v>
       </c>
       <c r="G25" s="8">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="H25" s="8">
         <v>3</v>
@@ -4758,7 +4758,7 @@
         <v>259</v>
       </c>
       <c r="G26" s="8">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="H26" s="8">
         <v>2</v>
@@ -4910,7 +4910,7 @@
         <v>240</v>
       </c>
       <c r="G30" s="8">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="H30" s="8">
         <v>5</v>
@@ -4948,7 +4948,7 @@
         <v>384</v>
       </c>
       <c r="G31" s="13">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="H31" s="13">
         <v>12</v>

</xml_diff>